<commit_message>
updates to code and data
</commit_message>
<xml_diff>
--- a/Week6/dictionary/c2021_b.xlsx
+++ b/Week6/dictionary/c2021_b.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shares\IPEDS\DCT\2021\Fall\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidtorres/Code/NU/TIM7020/Week6/dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D8BF04-56D1-E94E-A70F-33552A283BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="330" windowWidth="12300" windowHeight="11640"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="12300" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="6" r:id="rId1"/>
@@ -487,9 +488,6 @@
     <t xml:space="preserve">This file contains the number of students who completed any degree or certificate by race/ethnicity and gender. Data covers all awards granted between July 1, 2020 and June 30, 2021. This file contains one record per institution. Each record is uniquely defined by the variables IPEDS ID (UNITID).  Each record will contain the total number of students,  men and women, and the total number of students for men and women for all nine race/ethnicity categories. </t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Number of students receiving awards/degrees conferred between July 1, 2020 and June 30, 2021 to all recipients, across all race/ethnicities and both genders</t>
   </si>
   <si>
@@ -604,16 +602,19 @@
   <si>
     <t>Number of nonresident alien women receiving awards/degrees  conferred between July 1, 2020 June 30, 2021. 
 Nonresident alien  - A person who is not a citizen or national of the United States and who is in this country on a visa or temporary basis and does not have the right to remain indefinitely.</t>
+  </si>
+  <si>
+    <t>PK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -711,7 +712,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -757,7 +758,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,9 +774,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -813,9 +814,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -850,7 +851,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -885,7 +886,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1058,21 +1059,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="24" t="s">
         <v>149</v>
       </c>
@@ -1086,7 +1087,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="27" t="s">
         <v>147</v>
       </c>
@@ -1100,7 +1101,7 @@
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="8"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1112,7 +1113,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1120,10 +1121,10 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="74.25" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1139,7 +1140,7 @@
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
     </row>
-    <row r="7" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="84" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1156,7 @@
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="26" t="s">
         <v>3</v>
       </c>
@@ -1169,7 +1170,7 @@
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
     </row>
-    <row r="11" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="77.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -1185,7 +1186,7 @@
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1201,7 +1202,7 @@
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
     </row>
-    <row r="13" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="26.25" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -1217,7 +1218,7 @@
       <c r="I13" s="23"/>
       <c r="J13" s="23"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>117</v>
       </c>
@@ -1251,26 +1252,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="13" style="22" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="13" style="22" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="107" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="15" customFormat="1">
       <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -1310,13 +1311,13 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="21">
         <v>33100</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="21">
         <v>33101</v>
       </c>
@@ -1362,7 +1363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="21">
         <v>33102</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="21">
         <v>33110</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="21">
         <v>33111</v>
       </c>
@@ -1431,7 +1432,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="21">
         <v>33112</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="21">
         <v>33120</v>
       </c>
@@ -1477,7 +1478,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="21">
         <v>33121</v>
       </c>
@@ -1500,7 +1501,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="21">
         <v>33122</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="21">
         <v>33130</v>
       </c>
@@ -1546,7 +1547,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="21">
         <v>33131</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="21">
         <v>33132</v>
       </c>
@@ -1592,7 +1593,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="21">
         <v>33140</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="21">
         <v>33141</v>
       </c>
@@ -1638,7 +1639,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="21">
         <v>33142</v>
       </c>
@@ -1661,7 +1662,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="21">
         <v>33150</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="21">
         <v>33151</v>
       </c>
@@ -1707,7 +1708,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="21">
         <v>33152</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="21">
         <v>33160</v>
       </c>
@@ -1753,7 +1754,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="21">
         <v>33161</v>
       </c>
@@ -1776,7 +1777,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="21">
         <v>33162</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="21">
         <v>33170</v>
       </c>
@@ -1822,7 +1823,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="21">
         <v>33171</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="21">
         <v>33172</v>
       </c>
@@ -1868,7 +1869,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="21">
         <v>33180</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="21">
         <v>33181</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="21">
         <v>33182</v>
       </c>
@@ -1937,7 +1938,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="21">
         <v>33190</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="21">
         <v>33191</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="21">
         <v>33192</v>
       </c>
@@ -2006,7 +2007,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="21"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2015,7 +2016,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="21"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2024,7 +2025,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="21"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2033,7 +2034,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="21"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2042,7 +2043,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="21"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2051,7 +2052,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="21"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2060,7 +2061,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="21"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2069,7 +2070,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="21"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2078,7 +2079,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="21"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2087,7 +2088,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="21"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2095,7 +2096,7 @@
       <c r="E42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="21"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2104,7 +2105,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="21"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2113,7 +2114,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="21"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2122,7 +2123,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="21"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2130,7 +2131,7 @@
       <c r="E46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="21"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2139,7 +2140,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="21"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2147,7 +2148,7 @@
       <c r="E48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" s="21"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2156,7 +2157,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" s="21"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2165,7 +2166,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" s="21"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2174,7 +2175,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" s="21"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2182,7 +2183,7 @@
       <c r="E52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" s="21"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2191,7 +2192,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" s="21"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2199,7 +2200,7 @@
       <c r="E54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" s="21"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2208,7 +2209,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" s="21"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2217,7 +2218,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" s="21"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2226,7 +2227,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" s="21"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2234,7 +2235,7 @@
       <c r="E58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" s="21"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2243,7 +2244,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" s="21"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2251,7 +2252,7 @@
       <c r="E60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" s="21"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2260,7 +2261,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" s="21"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2269,7 +2270,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" s="21"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2278,7 +2279,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" s="21"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2287,7 +2288,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" s="21"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2296,7 +2297,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" s="21"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2305,7 +2306,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" s="21"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2314,7 +2315,7 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" s="21"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2323,7 +2324,7 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" s="21"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2332,7 +2333,7 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" s="21"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2341,7 +2342,7 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" s="21"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2350,7 +2351,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" s="21"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2359,7 +2360,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" s="21"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2368,7 +2369,7 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" s="21"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2377,7 +2378,7 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" s="21"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2386,7 +2387,7 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" s="21"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2395,7 +2396,7 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" s="21"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2404,7 +2405,7 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" s="21"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2413,7 +2414,7 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" s="21"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2422,7 +2423,7 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" s="21"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2431,7 +2432,7 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7">
       <c r="A81" s="21"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2440,7 +2441,7 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7">
       <c r="A82" s="21"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2449,7 +2450,7 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7">
       <c r="A83" s="21"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2458,7 +2459,7 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84" s="21"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2467,7 +2468,7 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7">
       <c r="A85" s="21"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2476,7 +2477,7 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7">
       <c r="A86" s="21"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2485,7 +2486,7 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87" s="21"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2494,7 +2495,7 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88" s="21"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2503,7 +2504,7 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7">
       <c r="A89" s="21"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2512,7 +2513,7 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7">
       <c r="A90" s="21"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2521,7 +2522,7 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7">
       <c r="A91" s="21"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2530,7 +2531,7 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7">
       <c r="A92" s="21"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2539,7 +2540,7 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="A93" s="21"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2548,7 +2549,7 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7">
       <c r="A94" s="21"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2557,7 +2558,7 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95" s="21"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2566,7 +2567,7 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7">
       <c r="A96" s="21"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2575,7 +2576,7 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" s="21"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2584,7 +2585,7 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98" s="21"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2593,7 +2594,7 @@
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7">
       <c r="A99" s="21"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2602,7 +2603,7 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7">
       <c r="A100" s="21"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2611,7 +2612,7 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101" s="21"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2620,7 +2621,7 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7">
       <c r="A102" s="21"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2629,7 +2630,7 @@
       <c r="F102" s="19"/>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="A103" s="21"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2637,7 +2638,7 @@
       <c r="E103" s="1"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104" s="21"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2645,7 +2646,7 @@
       <c r="E104" s="1"/>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105" s="21"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2654,7 +2655,7 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106" s="21"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2663,7 +2664,7 @@
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7">
       <c r="A107" s="21"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2672,7 +2673,7 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108" s="21"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2681,7 +2682,7 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7">
       <c r="A109" s="21"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2690,7 +2691,7 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110" s="21"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2699,7 +2700,7 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7">
       <c r="A111" s="21"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2708,7 +2709,7 @@
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7">
       <c r="A112" s="21"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2717,7 +2718,7 @@
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7">
       <c r="A113" s="21"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2725,7 +2726,7 @@
       <c r="E113" s="1"/>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7">
       <c r="A114" s="21"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2734,7 +2735,7 @@
       <c r="F114" s="19"/>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7">
       <c r="A115" s="21"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2742,7 +2743,7 @@
       <c r="E115" s="1"/>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7">
       <c r="A116" s="21"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2750,7 +2751,7 @@
       <c r="E116" s="1"/>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7">
       <c r="A117" s="21"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2758,7 +2759,7 @@
       <c r="E117" s="1"/>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7">
       <c r="A118" s="21"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2766,7 +2767,7 @@
       <c r="E118" s="1"/>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7">
       <c r="A119" s="21"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2775,7 +2776,7 @@
       <c r="F119" s="19"/>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7">
       <c r="A120" s="21"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2783,7 +2784,7 @@
       <c r="E120" s="1"/>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7">
       <c r="A121" s="21"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2791,7 +2792,7 @@
       <c r="E121" s="1"/>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7">
       <c r="A122" s="21"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2799,7 +2800,7 @@
       <c r="E122" s="1"/>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7">
       <c r="A123" s="21"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2807,7 +2808,7 @@
       <c r="E123" s="1"/>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7">
       <c r="A124" s="21"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2815,7 +2816,7 @@
       <c r="E124" s="1"/>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7">
       <c r="A125" s="21"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2823,7 +2824,7 @@
       <c r="E125" s="1"/>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7">
       <c r="A126" s="21"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2831,7 +2832,7 @@
       <c r="E126" s="1"/>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7">
       <c r="A127" s="21"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2840,7 +2841,7 @@
       <c r="F127" s="19"/>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7">
       <c r="A128" s="21"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2849,7 +2850,7 @@
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7">
       <c r="A129" s="21"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2858,7 +2859,7 @@
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7">
       <c r="A130" s="21"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2867,7 +2868,7 @@
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7">
       <c r="A131" s="21"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2876,7 +2877,7 @@
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7">
       <c r="A132" s="21"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2885,7 +2886,7 @@
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7">
       <c r="A133" s="21"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2893,7 +2894,7 @@
       <c r="E133" s="1"/>
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7">
       <c r="A134" s="21"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2902,7 +2903,7 @@
       <c r="F134" s="19"/>
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7">
       <c r="A135" s="21"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2911,7 +2912,7 @@
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7">
       <c r="A136" s="21"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2920,7 +2921,7 @@
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7">
       <c r="A137" s="21"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2929,7 +2930,7 @@
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7">
       <c r="A138" s="21"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2945,7 +2946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2953,204 +2954,204 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="11"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="11.140625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="144.85546875" style="13" customWidth="1"/>
-    <col min="4" max="257" width="9.140625" style="14"/>
-    <col min="258" max="258" width="11.140625" style="14" customWidth="1"/>
-    <col min="259" max="259" width="144.85546875" style="14" customWidth="1"/>
-    <col min="260" max="513" width="9.140625" style="14"/>
-    <col min="514" max="514" width="11.140625" style="14" customWidth="1"/>
-    <col min="515" max="515" width="144.85546875" style="14" customWidth="1"/>
-    <col min="516" max="769" width="9.140625" style="14"/>
-    <col min="770" max="770" width="11.140625" style="14" customWidth="1"/>
-    <col min="771" max="771" width="144.85546875" style="14" customWidth="1"/>
-    <col min="772" max="1025" width="9.140625" style="14"/>
-    <col min="1026" max="1026" width="11.140625" style="14" customWidth="1"/>
-    <col min="1027" max="1027" width="144.85546875" style="14" customWidth="1"/>
-    <col min="1028" max="1281" width="9.140625" style="14"/>
-    <col min="1282" max="1282" width="11.140625" style="14" customWidth="1"/>
-    <col min="1283" max="1283" width="144.85546875" style="14" customWidth="1"/>
-    <col min="1284" max="1537" width="9.140625" style="14"/>
-    <col min="1538" max="1538" width="11.140625" style="14" customWidth="1"/>
-    <col min="1539" max="1539" width="144.85546875" style="14" customWidth="1"/>
-    <col min="1540" max="1793" width="9.140625" style="14"/>
-    <col min="1794" max="1794" width="11.140625" style="14" customWidth="1"/>
-    <col min="1795" max="1795" width="144.85546875" style="14" customWidth="1"/>
-    <col min="1796" max="2049" width="9.140625" style="14"/>
-    <col min="2050" max="2050" width="11.140625" style="14" customWidth="1"/>
-    <col min="2051" max="2051" width="144.85546875" style="14" customWidth="1"/>
-    <col min="2052" max="2305" width="9.140625" style="14"/>
-    <col min="2306" max="2306" width="11.140625" style="14" customWidth="1"/>
-    <col min="2307" max="2307" width="144.85546875" style="14" customWidth="1"/>
-    <col min="2308" max="2561" width="9.140625" style="14"/>
-    <col min="2562" max="2562" width="11.140625" style="14" customWidth="1"/>
-    <col min="2563" max="2563" width="144.85546875" style="14" customWidth="1"/>
-    <col min="2564" max="2817" width="9.140625" style="14"/>
-    <col min="2818" max="2818" width="11.140625" style="14" customWidth="1"/>
-    <col min="2819" max="2819" width="144.85546875" style="14" customWidth="1"/>
-    <col min="2820" max="3073" width="9.140625" style="14"/>
-    <col min="3074" max="3074" width="11.140625" style="14" customWidth="1"/>
-    <col min="3075" max="3075" width="144.85546875" style="14" customWidth="1"/>
-    <col min="3076" max="3329" width="9.140625" style="14"/>
-    <col min="3330" max="3330" width="11.140625" style="14" customWidth="1"/>
-    <col min="3331" max="3331" width="144.85546875" style="14" customWidth="1"/>
-    <col min="3332" max="3585" width="9.140625" style="14"/>
-    <col min="3586" max="3586" width="11.140625" style="14" customWidth="1"/>
-    <col min="3587" max="3587" width="144.85546875" style="14" customWidth="1"/>
-    <col min="3588" max="3841" width="9.140625" style="14"/>
-    <col min="3842" max="3842" width="11.140625" style="14" customWidth="1"/>
-    <col min="3843" max="3843" width="144.85546875" style="14" customWidth="1"/>
-    <col min="3844" max="4097" width="9.140625" style="14"/>
-    <col min="4098" max="4098" width="11.140625" style="14" customWidth="1"/>
-    <col min="4099" max="4099" width="144.85546875" style="14" customWidth="1"/>
-    <col min="4100" max="4353" width="9.140625" style="14"/>
-    <col min="4354" max="4354" width="11.140625" style="14" customWidth="1"/>
-    <col min="4355" max="4355" width="144.85546875" style="14" customWidth="1"/>
-    <col min="4356" max="4609" width="9.140625" style="14"/>
-    <col min="4610" max="4610" width="11.140625" style="14" customWidth="1"/>
-    <col min="4611" max="4611" width="144.85546875" style="14" customWidth="1"/>
-    <col min="4612" max="4865" width="9.140625" style="14"/>
-    <col min="4866" max="4866" width="11.140625" style="14" customWidth="1"/>
-    <col min="4867" max="4867" width="144.85546875" style="14" customWidth="1"/>
-    <col min="4868" max="5121" width="9.140625" style="14"/>
-    <col min="5122" max="5122" width="11.140625" style="14" customWidth="1"/>
-    <col min="5123" max="5123" width="144.85546875" style="14" customWidth="1"/>
-    <col min="5124" max="5377" width="9.140625" style="14"/>
-    <col min="5378" max="5378" width="11.140625" style="14" customWidth="1"/>
-    <col min="5379" max="5379" width="144.85546875" style="14" customWidth="1"/>
-    <col min="5380" max="5633" width="9.140625" style="14"/>
-    <col min="5634" max="5634" width="11.140625" style="14" customWidth="1"/>
-    <col min="5635" max="5635" width="144.85546875" style="14" customWidth="1"/>
-    <col min="5636" max="5889" width="9.140625" style="14"/>
-    <col min="5890" max="5890" width="11.140625" style="14" customWidth="1"/>
-    <col min="5891" max="5891" width="144.85546875" style="14" customWidth="1"/>
-    <col min="5892" max="6145" width="9.140625" style="14"/>
-    <col min="6146" max="6146" width="11.140625" style="14" customWidth="1"/>
-    <col min="6147" max="6147" width="144.85546875" style="14" customWidth="1"/>
-    <col min="6148" max="6401" width="9.140625" style="14"/>
-    <col min="6402" max="6402" width="11.140625" style="14" customWidth="1"/>
-    <col min="6403" max="6403" width="144.85546875" style="14" customWidth="1"/>
-    <col min="6404" max="6657" width="9.140625" style="14"/>
-    <col min="6658" max="6658" width="11.140625" style="14" customWidth="1"/>
-    <col min="6659" max="6659" width="144.85546875" style="14" customWidth="1"/>
-    <col min="6660" max="6913" width="9.140625" style="14"/>
-    <col min="6914" max="6914" width="11.140625" style="14" customWidth="1"/>
-    <col min="6915" max="6915" width="144.85546875" style="14" customWidth="1"/>
-    <col min="6916" max="7169" width="9.140625" style="14"/>
-    <col min="7170" max="7170" width="11.140625" style="14" customWidth="1"/>
-    <col min="7171" max="7171" width="144.85546875" style="14" customWidth="1"/>
-    <col min="7172" max="7425" width="9.140625" style="14"/>
-    <col min="7426" max="7426" width="11.140625" style="14" customWidth="1"/>
-    <col min="7427" max="7427" width="144.85546875" style="14" customWidth="1"/>
-    <col min="7428" max="7681" width="9.140625" style="14"/>
-    <col min="7682" max="7682" width="11.140625" style="14" customWidth="1"/>
-    <col min="7683" max="7683" width="144.85546875" style="14" customWidth="1"/>
-    <col min="7684" max="7937" width="9.140625" style="14"/>
-    <col min="7938" max="7938" width="11.140625" style="14" customWidth="1"/>
-    <col min="7939" max="7939" width="144.85546875" style="14" customWidth="1"/>
-    <col min="7940" max="8193" width="9.140625" style="14"/>
-    <col min="8194" max="8194" width="11.140625" style="14" customWidth="1"/>
-    <col min="8195" max="8195" width="144.85546875" style="14" customWidth="1"/>
-    <col min="8196" max="8449" width="9.140625" style="14"/>
-    <col min="8450" max="8450" width="11.140625" style="14" customWidth="1"/>
-    <col min="8451" max="8451" width="144.85546875" style="14" customWidth="1"/>
-    <col min="8452" max="8705" width="9.140625" style="14"/>
-    <col min="8706" max="8706" width="11.140625" style="14" customWidth="1"/>
-    <col min="8707" max="8707" width="144.85546875" style="14" customWidth="1"/>
-    <col min="8708" max="8961" width="9.140625" style="14"/>
-    <col min="8962" max="8962" width="11.140625" style="14" customWidth="1"/>
-    <col min="8963" max="8963" width="144.85546875" style="14" customWidth="1"/>
-    <col min="8964" max="9217" width="9.140625" style="14"/>
-    <col min="9218" max="9218" width="11.140625" style="14" customWidth="1"/>
-    <col min="9219" max="9219" width="144.85546875" style="14" customWidth="1"/>
-    <col min="9220" max="9473" width="9.140625" style="14"/>
-    <col min="9474" max="9474" width="11.140625" style="14" customWidth="1"/>
-    <col min="9475" max="9475" width="144.85546875" style="14" customWidth="1"/>
-    <col min="9476" max="9729" width="9.140625" style="14"/>
-    <col min="9730" max="9730" width="11.140625" style="14" customWidth="1"/>
-    <col min="9731" max="9731" width="144.85546875" style="14" customWidth="1"/>
-    <col min="9732" max="9985" width="9.140625" style="14"/>
-    <col min="9986" max="9986" width="11.140625" style="14" customWidth="1"/>
-    <col min="9987" max="9987" width="144.85546875" style="14" customWidth="1"/>
-    <col min="9988" max="10241" width="9.140625" style="14"/>
-    <col min="10242" max="10242" width="11.140625" style="14" customWidth="1"/>
-    <col min="10243" max="10243" width="144.85546875" style="14" customWidth="1"/>
-    <col min="10244" max="10497" width="9.140625" style="14"/>
-    <col min="10498" max="10498" width="11.140625" style="14" customWidth="1"/>
-    <col min="10499" max="10499" width="144.85546875" style="14" customWidth="1"/>
-    <col min="10500" max="10753" width="9.140625" style="14"/>
-    <col min="10754" max="10754" width="11.140625" style="14" customWidth="1"/>
-    <col min="10755" max="10755" width="144.85546875" style="14" customWidth="1"/>
-    <col min="10756" max="11009" width="9.140625" style="14"/>
-    <col min="11010" max="11010" width="11.140625" style="14" customWidth="1"/>
-    <col min="11011" max="11011" width="144.85546875" style="14" customWidth="1"/>
-    <col min="11012" max="11265" width="9.140625" style="14"/>
-    <col min="11266" max="11266" width="11.140625" style="14" customWidth="1"/>
-    <col min="11267" max="11267" width="144.85546875" style="14" customWidth="1"/>
-    <col min="11268" max="11521" width="9.140625" style="14"/>
-    <col min="11522" max="11522" width="11.140625" style="14" customWidth="1"/>
-    <col min="11523" max="11523" width="144.85546875" style="14" customWidth="1"/>
-    <col min="11524" max="11777" width="9.140625" style="14"/>
-    <col min="11778" max="11778" width="11.140625" style="14" customWidth="1"/>
-    <col min="11779" max="11779" width="144.85546875" style="14" customWidth="1"/>
-    <col min="11780" max="12033" width="9.140625" style="14"/>
-    <col min="12034" max="12034" width="11.140625" style="14" customWidth="1"/>
-    <col min="12035" max="12035" width="144.85546875" style="14" customWidth="1"/>
-    <col min="12036" max="12289" width="9.140625" style="14"/>
-    <col min="12290" max="12290" width="11.140625" style="14" customWidth="1"/>
-    <col min="12291" max="12291" width="144.85546875" style="14" customWidth="1"/>
-    <col min="12292" max="12545" width="9.140625" style="14"/>
-    <col min="12546" max="12546" width="11.140625" style="14" customWidth="1"/>
-    <col min="12547" max="12547" width="144.85546875" style="14" customWidth="1"/>
-    <col min="12548" max="12801" width="9.140625" style="14"/>
-    <col min="12802" max="12802" width="11.140625" style="14" customWidth="1"/>
-    <col min="12803" max="12803" width="144.85546875" style="14" customWidth="1"/>
-    <col min="12804" max="13057" width="9.140625" style="14"/>
-    <col min="13058" max="13058" width="11.140625" style="14" customWidth="1"/>
-    <col min="13059" max="13059" width="144.85546875" style="14" customWidth="1"/>
-    <col min="13060" max="13313" width="9.140625" style="14"/>
-    <col min="13314" max="13314" width="11.140625" style="14" customWidth="1"/>
-    <col min="13315" max="13315" width="144.85546875" style="14" customWidth="1"/>
-    <col min="13316" max="13569" width="9.140625" style="14"/>
-    <col min="13570" max="13570" width="11.140625" style="14" customWidth="1"/>
-    <col min="13571" max="13571" width="144.85546875" style="14" customWidth="1"/>
-    <col min="13572" max="13825" width="9.140625" style="14"/>
-    <col min="13826" max="13826" width="11.140625" style="14" customWidth="1"/>
-    <col min="13827" max="13827" width="144.85546875" style="14" customWidth="1"/>
-    <col min="13828" max="14081" width="9.140625" style="14"/>
-    <col min="14082" max="14082" width="11.140625" style="14" customWidth="1"/>
-    <col min="14083" max="14083" width="144.85546875" style="14" customWidth="1"/>
-    <col min="14084" max="14337" width="9.140625" style="14"/>
-    <col min="14338" max="14338" width="11.140625" style="14" customWidth="1"/>
-    <col min="14339" max="14339" width="144.85546875" style="14" customWidth="1"/>
-    <col min="14340" max="14593" width="9.140625" style="14"/>
-    <col min="14594" max="14594" width="11.140625" style="14" customWidth="1"/>
-    <col min="14595" max="14595" width="144.85546875" style="14" customWidth="1"/>
-    <col min="14596" max="14849" width="9.140625" style="14"/>
-    <col min="14850" max="14850" width="11.140625" style="14" customWidth="1"/>
-    <col min="14851" max="14851" width="144.85546875" style="14" customWidth="1"/>
-    <col min="14852" max="15105" width="9.140625" style="14"/>
-    <col min="15106" max="15106" width="11.140625" style="14" customWidth="1"/>
-    <col min="15107" max="15107" width="144.85546875" style="14" customWidth="1"/>
-    <col min="15108" max="15361" width="9.140625" style="14"/>
-    <col min="15362" max="15362" width="11.140625" style="14" customWidth="1"/>
-    <col min="15363" max="15363" width="144.85546875" style="14" customWidth="1"/>
-    <col min="15364" max="15617" width="9.140625" style="14"/>
-    <col min="15618" max="15618" width="11.140625" style="14" customWidth="1"/>
-    <col min="15619" max="15619" width="144.85546875" style="14" customWidth="1"/>
-    <col min="15620" max="15873" width="9.140625" style="14"/>
-    <col min="15874" max="15874" width="11.140625" style="14" customWidth="1"/>
-    <col min="15875" max="15875" width="144.85546875" style="14" customWidth="1"/>
-    <col min="15876" max="16129" width="9.140625" style="14"/>
-    <col min="16130" max="16130" width="11.140625" style="14" customWidth="1"/>
-    <col min="16131" max="16131" width="144.85546875" style="14" customWidth="1"/>
-    <col min="16132" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="1" width="9.19921875" style="13"/>
+    <col min="2" max="2" width="11.19921875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="144.796875" style="13" customWidth="1"/>
+    <col min="4" max="257" width="9.19921875" style="14"/>
+    <col min="258" max="258" width="11.19921875" style="14" customWidth="1"/>
+    <col min="259" max="259" width="144.796875" style="14" customWidth="1"/>
+    <col min="260" max="513" width="9.19921875" style="14"/>
+    <col min="514" max="514" width="11.19921875" style="14" customWidth="1"/>
+    <col min="515" max="515" width="144.796875" style="14" customWidth="1"/>
+    <col min="516" max="769" width="9.19921875" style="14"/>
+    <col min="770" max="770" width="11.19921875" style="14" customWidth="1"/>
+    <col min="771" max="771" width="144.796875" style="14" customWidth="1"/>
+    <col min="772" max="1025" width="9.19921875" style="14"/>
+    <col min="1026" max="1026" width="11.19921875" style="14" customWidth="1"/>
+    <col min="1027" max="1027" width="144.796875" style="14" customWidth="1"/>
+    <col min="1028" max="1281" width="9.19921875" style="14"/>
+    <col min="1282" max="1282" width="11.19921875" style="14" customWidth="1"/>
+    <col min="1283" max="1283" width="144.796875" style="14" customWidth="1"/>
+    <col min="1284" max="1537" width="9.19921875" style="14"/>
+    <col min="1538" max="1538" width="11.19921875" style="14" customWidth="1"/>
+    <col min="1539" max="1539" width="144.796875" style="14" customWidth="1"/>
+    <col min="1540" max="1793" width="9.19921875" style="14"/>
+    <col min="1794" max="1794" width="11.19921875" style="14" customWidth="1"/>
+    <col min="1795" max="1795" width="144.796875" style="14" customWidth="1"/>
+    <col min="1796" max="2049" width="9.19921875" style="14"/>
+    <col min="2050" max="2050" width="11.19921875" style="14" customWidth="1"/>
+    <col min="2051" max="2051" width="144.796875" style="14" customWidth="1"/>
+    <col min="2052" max="2305" width="9.19921875" style="14"/>
+    <col min="2306" max="2306" width="11.19921875" style="14" customWidth="1"/>
+    <col min="2307" max="2307" width="144.796875" style="14" customWidth="1"/>
+    <col min="2308" max="2561" width="9.19921875" style="14"/>
+    <col min="2562" max="2562" width="11.19921875" style="14" customWidth="1"/>
+    <col min="2563" max="2563" width="144.796875" style="14" customWidth="1"/>
+    <col min="2564" max="2817" width="9.19921875" style="14"/>
+    <col min="2818" max="2818" width="11.19921875" style="14" customWidth="1"/>
+    <col min="2819" max="2819" width="144.796875" style="14" customWidth="1"/>
+    <col min="2820" max="3073" width="9.19921875" style="14"/>
+    <col min="3074" max="3074" width="11.19921875" style="14" customWidth="1"/>
+    <col min="3075" max="3075" width="144.796875" style="14" customWidth="1"/>
+    <col min="3076" max="3329" width="9.19921875" style="14"/>
+    <col min="3330" max="3330" width="11.19921875" style="14" customWidth="1"/>
+    <col min="3331" max="3331" width="144.796875" style="14" customWidth="1"/>
+    <col min="3332" max="3585" width="9.19921875" style="14"/>
+    <col min="3586" max="3586" width="11.19921875" style="14" customWidth="1"/>
+    <col min="3587" max="3587" width="144.796875" style="14" customWidth="1"/>
+    <col min="3588" max="3841" width="9.19921875" style="14"/>
+    <col min="3842" max="3842" width="11.19921875" style="14" customWidth="1"/>
+    <col min="3843" max="3843" width="144.796875" style="14" customWidth="1"/>
+    <col min="3844" max="4097" width="9.19921875" style="14"/>
+    <col min="4098" max="4098" width="11.19921875" style="14" customWidth="1"/>
+    <col min="4099" max="4099" width="144.796875" style="14" customWidth="1"/>
+    <col min="4100" max="4353" width="9.19921875" style="14"/>
+    <col min="4354" max="4354" width="11.19921875" style="14" customWidth="1"/>
+    <col min="4355" max="4355" width="144.796875" style="14" customWidth="1"/>
+    <col min="4356" max="4609" width="9.19921875" style="14"/>
+    <col min="4610" max="4610" width="11.19921875" style="14" customWidth="1"/>
+    <col min="4611" max="4611" width="144.796875" style="14" customWidth="1"/>
+    <col min="4612" max="4865" width="9.19921875" style="14"/>
+    <col min="4866" max="4866" width="11.19921875" style="14" customWidth="1"/>
+    <col min="4867" max="4867" width="144.796875" style="14" customWidth="1"/>
+    <col min="4868" max="5121" width="9.19921875" style="14"/>
+    <col min="5122" max="5122" width="11.19921875" style="14" customWidth="1"/>
+    <col min="5123" max="5123" width="144.796875" style="14" customWidth="1"/>
+    <col min="5124" max="5377" width="9.19921875" style="14"/>
+    <col min="5378" max="5378" width="11.19921875" style="14" customWidth="1"/>
+    <col min="5379" max="5379" width="144.796875" style="14" customWidth="1"/>
+    <col min="5380" max="5633" width="9.19921875" style="14"/>
+    <col min="5634" max="5634" width="11.19921875" style="14" customWidth="1"/>
+    <col min="5635" max="5635" width="144.796875" style="14" customWidth="1"/>
+    <col min="5636" max="5889" width="9.19921875" style="14"/>
+    <col min="5890" max="5890" width="11.19921875" style="14" customWidth="1"/>
+    <col min="5891" max="5891" width="144.796875" style="14" customWidth="1"/>
+    <col min="5892" max="6145" width="9.19921875" style="14"/>
+    <col min="6146" max="6146" width="11.19921875" style="14" customWidth="1"/>
+    <col min="6147" max="6147" width="144.796875" style="14" customWidth="1"/>
+    <col min="6148" max="6401" width="9.19921875" style="14"/>
+    <col min="6402" max="6402" width="11.19921875" style="14" customWidth="1"/>
+    <col min="6403" max="6403" width="144.796875" style="14" customWidth="1"/>
+    <col min="6404" max="6657" width="9.19921875" style="14"/>
+    <col min="6658" max="6658" width="11.19921875" style="14" customWidth="1"/>
+    <col min="6659" max="6659" width="144.796875" style="14" customWidth="1"/>
+    <col min="6660" max="6913" width="9.19921875" style="14"/>
+    <col min="6914" max="6914" width="11.19921875" style="14" customWidth="1"/>
+    <col min="6915" max="6915" width="144.796875" style="14" customWidth="1"/>
+    <col min="6916" max="7169" width="9.19921875" style="14"/>
+    <col min="7170" max="7170" width="11.19921875" style="14" customWidth="1"/>
+    <col min="7171" max="7171" width="144.796875" style="14" customWidth="1"/>
+    <col min="7172" max="7425" width="9.19921875" style="14"/>
+    <col min="7426" max="7426" width="11.19921875" style="14" customWidth="1"/>
+    <col min="7427" max="7427" width="144.796875" style="14" customWidth="1"/>
+    <col min="7428" max="7681" width="9.19921875" style="14"/>
+    <col min="7682" max="7682" width="11.19921875" style="14" customWidth="1"/>
+    <col min="7683" max="7683" width="144.796875" style="14" customWidth="1"/>
+    <col min="7684" max="7937" width="9.19921875" style="14"/>
+    <col min="7938" max="7938" width="11.19921875" style="14" customWidth="1"/>
+    <col min="7939" max="7939" width="144.796875" style="14" customWidth="1"/>
+    <col min="7940" max="8193" width="9.19921875" style="14"/>
+    <col min="8194" max="8194" width="11.19921875" style="14" customWidth="1"/>
+    <col min="8195" max="8195" width="144.796875" style="14" customWidth="1"/>
+    <col min="8196" max="8449" width="9.19921875" style="14"/>
+    <col min="8450" max="8450" width="11.19921875" style="14" customWidth="1"/>
+    <col min="8451" max="8451" width="144.796875" style="14" customWidth="1"/>
+    <col min="8452" max="8705" width="9.19921875" style="14"/>
+    <col min="8706" max="8706" width="11.19921875" style="14" customWidth="1"/>
+    <col min="8707" max="8707" width="144.796875" style="14" customWidth="1"/>
+    <col min="8708" max="8961" width="9.19921875" style="14"/>
+    <col min="8962" max="8962" width="11.19921875" style="14" customWidth="1"/>
+    <col min="8963" max="8963" width="144.796875" style="14" customWidth="1"/>
+    <col min="8964" max="9217" width="9.19921875" style="14"/>
+    <col min="9218" max="9218" width="11.19921875" style="14" customWidth="1"/>
+    <col min="9219" max="9219" width="144.796875" style="14" customWidth="1"/>
+    <col min="9220" max="9473" width="9.19921875" style="14"/>
+    <col min="9474" max="9474" width="11.19921875" style="14" customWidth="1"/>
+    <col min="9475" max="9475" width="144.796875" style="14" customWidth="1"/>
+    <col min="9476" max="9729" width="9.19921875" style="14"/>
+    <col min="9730" max="9730" width="11.19921875" style="14" customWidth="1"/>
+    <col min="9731" max="9731" width="144.796875" style="14" customWidth="1"/>
+    <col min="9732" max="9985" width="9.19921875" style="14"/>
+    <col min="9986" max="9986" width="11.19921875" style="14" customWidth="1"/>
+    <col min="9987" max="9987" width="144.796875" style="14" customWidth="1"/>
+    <col min="9988" max="10241" width="9.19921875" style="14"/>
+    <col min="10242" max="10242" width="11.19921875" style="14" customWidth="1"/>
+    <col min="10243" max="10243" width="144.796875" style="14" customWidth="1"/>
+    <col min="10244" max="10497" width="9.19921875" style="14"/>
+    <col min="10498" max="10498" width="11.19921875" style="14" customWidth="1"/>
+    <col min="10499" max="10499" width="144.796875" style="14" customWidth="1"/>
+    <col min="10500" max="10753" width="9.19921875" style="14"/>
+    <col min="10754" max="10754" width="11.19921875" style="14" customWidth="1"/>
+    <col min="10755" max="10755" width="144.796875" style="14" customWidth="1"/>
+    <col min="10756" max="11009" width="9.19921875" style="14"/>
+    <col min="11010" max="11010" width="11.19921875" style="14" customWidth="1"/>
+    <col min="11011" max="11011" width="144.796875" style="14" customWidth="1"/>
+    <col min="11012" max="11265" width="9.19921875" style="14"/>
+    <col min="11266" max="11266" width="11.19921875" style="14" customWidth="1"/>
+    <col min="11267" max="11267" width="144.796875" style="14" customWidth="1"/>
+    <col min="11268" max="11521" width="9.19921875" style="14"/>
+    <col min="11522" max="11522" width="11.19921875" style="14" customWidth="1"/>
+    <col min="11523" max="11523" width="144.796875" style="14" customWidth="1"/>
+    <col min="11524" max="11777" width="9.19921875" style="14"/>
+    <col min="11778" max="11778" width="11.19921875" style="14" customWidth="1"/>
+    <col min="11779" max="11779" width="144.796875" style="14" customWidth="1"/>
+    <col min="11780" max="12033" width="9.19921875" style="14"/>
+    <col min="12034" max="12034" width="11.19921875" style="14" customWidth="1"/>
+    <col min="12035" max="12035" width="144.796875" style="14" customWidth="1"/>
+    <col min="12036" max="12289" width="9.19921875" style="14"/>
+    <col min="12290" max="12290" width="11.19921875" style="14" customWidth="1"/>
+    <col min="12291" max="12291" width="144.796875" style="14" customWidth="1"/>
+    <col min="12292" max="12545" width="9.19921875" style="14"/>
+    <col min="12546" max="12546" width="11.19921875" style="14" customWidth="1"/>
+    <col min="12547" max="12547" width="144.796875" style="14" customWidth="1"/>
+    <col min="12548" max="12801" width="9.19921875" style="14"/>
+    <col min="12802" max="12802" width="11.19921875" style="14" customWidth="1"/>
+    <col min="12803" max="12803" width="144.796875" style="14" customWidth="1"/>
+    <col min="12804" max="13057" width="9.19921875" style="14"/>
+    <col min="13058" max="13058" width="11.19921875" style="14" customWidth="1"/>
+    <col min="13059" max="13059" width="144.796875" style="14" customWidth="1"/>
+    <col min="13060" max="13313" width="9.19921875" style="14"/>
+    <col min="13314" max="13314" width="11.19921875" style="14" customWidth="1"/>
+    <col min="13315" max="13315" width="144.796875" style="14" customWidth="1"/>
+    <col min="13316" max="13569" width="9.19921875" style="14"/>
+    <col min="13570" max="13570" width="11.19921875" style="14" customWidth="1"/>
+    <col min="13571" max="13571" width="144.796875" style="14" customWidth="1"/>
+    <col min="13572" max="13825" width="9.19921875" style="14"/>
+    <col min="13826" max="13826" width="11.19921875" style="14" customWidth="1"/>
+    <col min="13827" max="13827" width="144.796875" style="14" customWidth="1"/>
+    <col min="13828" max="14081" width="9.19921875" style="14"/>
+    <col min="14082" max="14082" width="11.19921875" style="14" customWidth="1"/>
+    <col min="14083" max="14083" width="144.796875" style="14" customWidth="1"/>
+    <col min="14084" max="14337" width="9.19921875" style="14"/>
+    <col min="14338" max="14338" width="11.19921875" style="14" customWidth="1"/>
+    <col min="14339" max="14339" width="144.796875" style="14" customWidth="1"/>
+    <col min="14340" max="14593" width="9.19921875" style="14"/>
+    <col min="14594" max="14594" width="11.19921875" style="14" customWidth="1"/>
+    <col min="14595" max="14595" width="144.796875" style="14" customWidth="1"/>
+    <col min="14596" max="14849" width="9.19921875" style="14"/>
+    <col min="14850" max="14850" width="11.19921875" style="14" customWidth="1"/>
+    <col min="14851" max="14851" width="144.796875" style="14" customWidth="1"/>
+    <col min="14852" max="15105" width="9.19921875" style="14"/>
+    <col min="15106" max="15106" width="11.19921875" style="14" customWidth="1"/>
+    <col min="15107" max="15107" width="144.796875" style="14" customWidth="1"/>
+    <col min="15108" max="15361" width="9.19921875" style="14"/>
+    <col min="15362" max="15362" width="11.19921875" style="14" customWidth="1"/>
+    <col min="15363" max="15363" width="144.796875" style="14" customWidth="1"/>
+    <col min="15364" max="15617" width="9.19921875" style="14"/>
+    <col min="15618" max="15618" width="11.19921875" style="14" customWidth="1"/>
+    <col min="15619" max="15619" width="144.796875" style="14" customWidth="1"/>
+    <col min="15620" max="15873" width="9.19921875" style="14"/>
+    <col min="15874" max="15874" width="11.19921875" style="14" customWidth="1"/>
+    <col min="15875" max="15875" width="144.796875" style="14" customWidth="1"/>
+    <col min="15876" max="16129" width="9.19921875" style="14"/>
+    <col min="16130" max="16130" width="11.19921875" style="14" customWidth="1"/>
+    <col min="16131" max="16131" width="144.796875" style="14" customWidth="1"/>
+    <col min="16132" max="16384" width="9.19921875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="12" customFormat="1" ht="12">
       <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
@@ -3161,7 +3162,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -3172,7 +3173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="12">
       <c r="A3" s="13">
         <v>33100</v>
       </c>
@@ -3180,10 +3181,10 @@
         <v>19</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="12">
       <c r="A4" s="13">
         <v>33101</v>
       </c>
@@ -3191,10 +3192,10 @@
         <v>22</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12">
       <c r="A5" s="13">
         <v>33102</v>
       </c>
@@ -3202,10 +3203,10 @@
         <v>25</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="48">
       <c r="A6" s="13">
         <v>33110</v>
       </c>
@@ -3213,10 +3214,10 @@
         <v>28</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="48">
       <c r="A7" s="13">
         <v>33111</v>
       </c>
@@ -3224,10 +3225,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="48">
       <c r="A8" s="13">
         <v>33112</v>
       </c>
@@ -3235,10 +3236,10 @@
         <v>34</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="48">
       <c r="A9" s="13">
         <v>33120</v>
       </c>
@@ -3246,10 +3247,10 @@
         <v>37</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="48">
       <c r="A10" s="13">
         <v>33121</v>
       </c>
@@ -3257,10 +3258,10 @@
         <v>40</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="48">
       <c r="A11" s="13">
         <v>33122</v>
       </c>
@@ -3268,10 +3269,10 @@
         <v>43</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="36">
       <c r="A12" s="13">
         <v>33130</v>
       </c>
@@ -3279,10 +3280,10 @@
         <v>46</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="36">
       <c r="A13" s="13">
         <v>33131</v>
       </c>
@@ -3290,10 +3291,10 @@
         <v>49</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="24">
       <c r="A14" s="13">
         <v>33132</v>
       </c>
@@ -3301,10 +3302,10 @@
         <v>52</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="36">
       <c r="A15" s="13">
         <v>33140</v>
       </c>
@@ -3312,10 +3313,10 @@
         <v>55</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="36">
       <c r="A16" s="13">
         <v>33141</v>
       </c>
@@ -3323,10 +3324,10 @@
         <v>58</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="36">
       <c r="A17" s="14">
         <v>33142</v>
       </c>
@@ -3334,10 +3335,10 @@
         <v>61</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="36">
       <c r="A18" s="14">
         <v>33150</v>
       </c>
@@ -3345,10 +3346,10 @@
         <v>64</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="36">
       <c r="A19" s="14">
         <v>33151</v>
       </c>
@@ -3356,10 +3357,10 @@
         <v>67</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="36">
       <c r="A20" s="14">
         <v>33152</v>
       </c>
@@ -3367,10 +3368,10 @@
         <v>70</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="36">
       <c r="A21" s="14">
         <v>33160</v>
       </c>
@@ -3378,10 +3379,10 @@
         <v>73</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="36">
       <c r="A22" s="14">
         <v>33161</v>
       </c>
@@ -3389,10 +3390,10 @@
         <v>76</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="36">
       <c r="A23" s="14">
         <v>33162</v>
       </c>
@@ -3400,10 +3401,10 @@
         <v>79</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="24">
       <c r="A24" s="14">
         <v>33170</v>
       </c>
@@ -3411,10 +3412,10 @@
         <v>82</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="36">
       <c r="A25" s="14">
         <v>33171</v>
       </c>
@@ -3422,10 +3423,10 @@
         <v>85</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="36">
       <c r="A26" s="14">
         <v>33172</v>
       </c>
@@ -3433,10 +3434,10 @@
         <v>88</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="36">
       <c r="A27" s="14">
         <v>33180</v>
       </c>
@@ -3444,10 +3445,10 @@
         <v>91</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="36">
       <c r="A28" s="14">
         <v>33181</v>
       </c>
@@ -3455,10 +3456,10 @@
         <v>94</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="36">
       <c r="A29" s="14">
         <v>33182</v>
       </c>
@@ -3466,10 +3467,10 @@
         <v>97</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="36">
       <c r="A30" s="14">
         <v>33190</v>
       </c>
@@ -3477,10 +3478,10 @@
         <v>100</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="36">
       <c r="A31" s="14">
         <v>33191</v>
       </c>
@@ -3488,10 +3489,10 @@
         <v>103</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="33.75" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="36">
       <c r="A32" s="14">
         <v>33192</v>
       </c>
@@ -3499,459 +3500,99 @@
         <v>106</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="14"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="14"/>
-      <c r="B78" s="14"/>
-      <c r="C78" s="14"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
-      <c r="B79" s="14"/>
-      <c r="C79" s="14"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="14"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="14"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="14"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="14"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="14"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="14"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="14"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="14"/>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="14"/>
-      <c r="B88" s="14"/>
-      <c r="C88" s="14"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="14"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="14"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="14"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="14"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="14"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="14"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="14"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="14"/>
-      <c r="B94" s="14"/>
-      <c r="C94" s="14"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="14"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="14"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="14"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="14"/>
-      <c r="B97" s="14"/>
-      <c r="C97" s="14"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="14"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="14"/>
-      <c r="B99" s="14"/>
-      <c r="C99" s="14"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="14"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="14"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="14"/>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="14"/>
-      <c r="B102" s="14"/>
-      <c r="C102" s="14"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="14"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="14"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="14"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="14"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="14"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="14"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="14"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="14"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="14"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="14"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="14"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="14"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="14"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="14"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="14"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="14"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="14"/>
-      <c r="B115" s="14"/>
-      <c r="C115" s="14"/>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="14"/>
-      <c r="B116" s="14"/>
-      <c r="C116" s="14"/>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="14"/>
-      <c r="B117" s="14"/>
-      <c r="C117" s="14"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="14"/>
-      <c r="B118" s="14"/>
-      <c r="C118" s="14"/>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="14"/>
-      <c r="B119" s="14"/>
-      <c r="C119" s="14"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="14"/>
-      <c r="B120" s="14"/>
-      <c r="C120" s="14"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" s="14"/>
-      <c r="B121" s="14"/>
-      <c r="C121" s="14"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" s="14"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="14"/>
-    </row>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" s="14" customFormat="1"/>
+    <row r="34" s="14" customFormat="1"/>
+    <row r="35" s="14" customFormat="1"/>
+    <row r="36" s="14" customFormat="1"/>
+    <row r="37" s="14" customFormat="1"/>
+    <row r="38" s="14" customFormat="1"/>
+    <row r="39" s="14" customFormat="1"/>
+    <row r="40" s="14" customFormat="1"/>
+    <row r="41" s="14" customFormat="1"/>
+    <row r="42" s="14" customFormat="1"/>
+    <row r="43" s="14" customFormat="1"/>
+    <row r="44" s="14" customFormat="1"/>
+    <row r="45" s="14" customFormat="1"/>
+    <row r="46" s="14" customFormat="1"/>
+    <row r="47" s="14" customFormat="1"/>
+    <row r="48" s="14" customFormat="1"/>
+    <row r="49" s="14" customFormat="1"/>
+    <row r="50" s="14" customFormat="1"/>
+    <row r="51" s="14" customFormat="1"/>
+    <row r="52" s="14" customFormat="1"/>
+    <row r="53" s="14" customFormat="1"/>
+    <row r="54" s="14" customFormat="1"/>
+    <row r="55" s="14" customFormat="1"/>
+    <row r="56" s="14" customFormat="1"/>
+    <row r="57" s="14" customFormat="1"/>
+    <row r="58" s="14" customFormat="1"/>
+    <row r="59" s="14" customFormat="1"/>
+    <row r="60" s="14" customFormat="1"/>
+    <row r="61" s="14" customFormat="1"/>
+    <row r="62" s="14" customFormat="1"/>
+    <row r="63" s="14" customFormat="1"/>
+    <row r="64" s="14" customFormat="1"/>
+    <row r="65" s="14" customFormat="1"/>
+    <row r="66" s="14" customFormat="1"/>
+    <row r="67" s="14" customFormat="1"/>
+    <row r="68" s="14" customFormat="1"/>
+    <row r="69" s="14" customFormat="1"/>
+    <row r="70" s="14" customFormat="1"/>
+    <row r="71" s="14" customFormat="1"/>
+    <row r="72" s="14" customFormat="1"/>
+    <row r="73" s="14" customFormat="1"/>
+    <row r="74" s="14" customFormat="1"/>
+    <row r="75" s="14" customFormat="1"/>
+    <row r="76" s="14" customFormat="1"/>
+    <row r="77" s="14" customFormat="1"/>
+    <row r="78" s="14" customFormat="1"/>
+    <row r="79" s="14" customFormat="1"/>
+    <row r="80" s="14" customFormat="1"/>
+    <row r="81" s="14" customFormat="1"/>
+    <row r="82" s="14" customFormat="1"/>
+    <row r="83" s="14" customFormat="1"/>
+    <row r="84" s="14" customFormat="1"/>
+    <row r="85" s="14" customFormat="1"/>
+    <row r="86" s="14" customFormat="1"/>
+    <row r="87" s="14" customFormat="1"/>
+    <row r="88" s="14" customFormat="1"/>
+    <row r="89" s="14" customFormat="1"/>
+    <row r="90" s="14" customFormat="1"/>
+    <row r="91" s="14" customFormat="1"/>
+    <row r="92" s="14" customFormat="1"/>
+    <row r="93" s="14" customFormat="1"/>
+    <row r="94" s="14" customFormat="1"/>
+    <row r="95" s="14" customFormat="1"/>
+    <row r="96" s="14" customFormat="1"/>
+    <row r="97" s="14" customFormat="1"/>
+    <row r="98" s="14" customFormat="1"/>
+    <row r="99" s="14" customFormat="1"/>
+    <row r="100" s="14" customFormat="1"/>
+    <row r="101" s="14" customFormat="1"/>
+    <row r="102" s="14" customFormat="1"/>
+    <row r="103" s="14" customFormat="1"/>
+    <row r="104" s="14" customFormat="1"/>
+    <row r="105" s="14" customFormat="1"/>
+    <row r="106" s="14" customFormat="1"/>
+    <row r="107" s="14" customFormat="1"/>
+    <row r="108" s="14" customFormat="1"/>
+    <row r="109" s="14" customFormat="1"/>
+    <row r="110" s="14" customFormat="1"/>
+    <row r="111" s="14" customFormat="1"/>
+    <row r="112" s="14" customFormat="1"/>
+    <row r="113" s="14" customFormat="1"/>
+    <row r="114" s="14" customFormat="1"/>
+    <row r="115" s="14" customFormat="1"/>
+    <row r="116" s="14" customFormat="1"/>
+    <row r="117" s="14" customFormat="1"/>
+    <row r="118" s="14" customFormat="1"/>
+    <row r="119" s="14" customFormat="1"/>
+    <row r="120" s="14" customFormat="1"/>
+    <row r="121" s="14" customFormat="1"/>
+    <row r="122" s="14" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
@@ -3959,7 +3600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3967,20 +3608,20 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="16" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="49.5703125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="49.59765625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4006,7 +3647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="10">
         <v>33100</v>
       </c>
@@ -4032,7 +3673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="10">
         <v>33101</v>
       </c>
@@ -4058,7 +3699,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="10">
         <v>33102</v>
       </c>
@@ -4084,7 +3725,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="10">
         <v>33110</v>
       </c>
@@ -4110,7 +3751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="10">
         <v>33111</v>
       </c>
@@ -4136,7 +3777,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="10">
         <v>33112</v>
       </c>
@@ -4162,7 +3803,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="10">
         <v>33120</v>
       </c>
@@ -4188,7 +3829,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="10">
         <v>33121</v>
       </c>
@@ -4214,7 +3855,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="10">
         <v>33122</v>
       </c>
@@ -4240,7 +3881,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="10">
         <v>33130</v>
       </c>
@@ -4266,7 +3907,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="10">
         <v>33131</v>
       </c>
@@ -4292,7 +3933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="10">
         <v>33132</v>
       </c>
@@ -4318,7 +3959,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="10">
         <v>33140</v>
       </c>
@@ -4344,7 +3985,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="10">
         <v>33141</v>
       </c>
@@ -4370,7 +4011,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="10">
         <v>33142</v>
       </c>
@@ -4396,7 +4037,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="10">
         <v>33150</v>
       </c>
@@ -4422,7 +4063,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="10">
         <v>33151</v>
       </c>
@@ -4448,7 +4089,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="10">
         <v>33152</v>
       </c>
@@ -4474,7 +4115,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="10">
         <v>33160</v>
       </c>
@@ -4500,7 +4141,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="10">
         <v>33161</v>
       </c>
@@ -4526,7 +4167,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="10">
         <v>33162</v>
       </c>
@@ -4552,7 +4193,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="10">
         <v>33170</v>
       </c>
@@ -4578,7 +4219,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="10">
         <v>33171</v>
       </c>
@@ -4604,7 +4245,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="10">
         <v>33172</v>
       </c>
@@ -4630,7 +4271,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="10">
         <v>33180</v>
       </c>
@@ -4656,7 +4297,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="10">
         <v>33181</v>
       </c>
@@ -4682,7 +4323,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="10">
         <v>33182</v>
       </c>
@@ -4708,7 +4349,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="10">
         <v>33190</v>
       </c>
@@ -4734,7 +4375,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" s="10">
         <v>33191</v>
       </c>
@@ -4760,7 +4401,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="10">
         <v>33192</v>
       </c>
@@ -4793,213 +4434,213 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="1" customWidth="1"/>
-    <col min="3" max="256" width="9.140625" style="1"/>
-    <col min="257" max="257" width="11.5703125" style="1" customWidth="1"/>
-    <col min="258" max="258" width="36.5703125" style="1" customWidth="1"/>
-    <col min="259" max="512" width="9.140625" style="1"/>
-    <col min="513" max="513" width="11.5703125" style="1" customWidth="1"/>
-    <col min="514" max="514" width="36.5703125" style="1" customWidth="1"/>
-    <col min="515" max="768" width="9.140625" style="1"/>
-    <col min="769" max="769" width="11.5703125" style="1" customWidth="1"/>
-    <col min="770" max="770" width="36.5703125" style="1" customWidth="1"/>
-    <col min="771" max="1024" width="9.140625" style="1"/>
-    <col min="1025" max="1025" width="11.5703125" style="1" customWidth="1"/>
-    <col min="1026" max="1026" width="36.5703125" style="1" customWidth="1"/>
-    <col min="1027" max="1280" width="9.140625" style="1"/>
-    <col min="1281" max="1281" width="11.5703125" style="1" customWidth="1"/>
-    <col min="1282" max="1282" width="36.5703125" style="1" customWidth="1"/>
-    <col min="1283" max="1536" width="9.140625" style="1"/>
-    <col min="1537" max="1537" width="11.5703125" style="1" customWidth="1"/>
-    <col min="1538" max="1538" width="36.5703125" style="1" customWidth="1"/>
-    <col min="1539" max="1792" width="9.140625" style="1"/>
-    <col min="1793" max="1793" width="11.5703125" style="1" customWidth="1"/>
-    <col min="1794" max="1794" width="36.5703125" style="1" customWidth="1"/>
-    <col min="1795" max="2048" width="9.140625" style="1"/>
-    <col min="2049" max="2049" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2050" max="2050" width="36.5703125" style="1" customWidth="1"/>
-    <col min="2051" max="2304" width="9.140625" style="1"/>
-    <col min="2305" max="2305" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2306" max="2306" width="36.5703125" style="1" customWidth="1"/>
-    <col min="2307" max="2560" width="9.140625" style="1"/>
-    <col min="2561" max="2561" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2562" max="2562" width="36.5703125" style="1" customWidth="1"/>
-    <col min="2563" max="2816" width="9.140625" style="1"/>
-    <col min="2817" max="2817" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2818" max="2818" width="36.5703125" style="1" customWidth="1"/>
-    <col min="2819" max="3072" width="9.140625" style="1"/>
-    <col min="3073" max="3073" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3074" max="3074" width="36.5703125" style="1" customWidth="1"/>
-    <col min="3075" max="3328" width="9.140625" style="1"/>
-    <col min="3329" max="3329" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3330" max="3330" width="36.5703125" style="1" customWidth="1"/>
-    <col min="3331" max="3584" width="9.140625" style="1"/>
-    <col min="3585" max="3585" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3586" max="3586" width="36.5703125" style="1" customWidth="1"/>
-    <col min="3587" max="3840" width="9.140625" style="1"/>
-    <col min="3841" max="3841" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3842" max="3842" width="36.5703125" style="1" customWidth="1"/>
-    <col min="3843" max="4096" width="9.140625" style="1"/>
-    <col min="4097" max="4097" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4098" max="4098" width="36.5703125" style="1" customWidth="1"/>
-    <col min="4099" max="4352" width="9.140625" style="1"/>
-    <col min="4353" max="4353" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4354" max="4354" width="36.5703125" style="1" customWidth="1"/>
-    <col min="4355" max="4608" width="9.140625" style="1"/>
-    <col min="4609" max="4609" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4610" max="4610" width="36.5703125" style="1" customWidth="1"/>
-    <col min="4611" max="4864" width="9.140625" style="1"/>
-    <col min="4865" max="4865" width="11.5703125" style="1" customWidth="1"/>
-    <col min="4866" max="4866" width="36.5703125" style="1" customWidth="1"/>
-    <col min="4867" max="5120" width="9.140625" style="1"/>
-    <col min="5121" max="5121" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5122" max="5122" width="36.5703125" style="1" customWidth="1"/>
-    <col min="5123" max="5376" width="9.140625" style="1"/>
-    <col min="5377" max="5377" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5378" max="5378" width="36.5703125" style="1" customWidth="1"/>
-    <col min="5379" max="5632" width="9.140625" style="1"/>
-    <col min="5633" max="5633" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5634" max="5634" width="36.5703125" style="1" customWidth="1"/>
-    <col min="5635" max="5888" width="9.140625" style="1"/>
-    <col min="5889" max="5889" width="11.5703125" style="1" customWidth="1"/>
-    <col min="5890" max="5890" width="36.5703125" style="1" customWidth="1"/>
-    <col min="5891" max="6144" width="9.140625" style="1"/>
-    <col min="6145" max="6145" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6146" max="6146" width="36.5703125" style="1" customWidth="1"/>
-    <col min="6147" max="6400" width="9.140625" style="1"/>
-    <col min="6401" max="6401" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6402" max="6402" width="36.5703125" style="1" customWidth="1"/>
-    <col min="6403" max="6656" width="9.140625" style="1"/>
-    <col min="6657" max="6657" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6658" max="6658" width="36.5703125" style="1" customWidth="1"/>
-    <col min="6659" max="6912" width="9.140625" style="1"/>
-    <col min="6913" max="6913" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6914" max="6914" width="36.5703125" style="1" customWidth="1"/>
-    <col min="6915" max="7168" width="9.140625" style="1"/>
-    <col min="7169" max="7169" width="11.5703125" style="1" customWidth="1"/>
-    <col min="7170" max="7170" width="36.5703125" style="1" customWidth="1"/>
-    <col min="7171" max="7424" width="9.140625" style="1"/>
-    <col min="7425" max="7425" width="11.5703125" style="1" customWidth="1"/>
-    <col min="7426" max="7426" width="36.5703125" style="1" customWidth="1"/>
-    <col min="7427" max="7680" width="9.140625" style="1"/>
-    <col min="7681" max="7681" width="11.5703125" style="1" customWidth="1"/>
-    <col min="7682" max="7682" width="36.5703125" style="1" customWidth="1"/>
-    <col min="7683" max="7936" width="9.140625" style="1"/>
-    <col min="7937" max="7937" width="11.5703125" style="1" customWidth="1"/>
-    <col min="7938" max="7938" width="36.5703125" style="1" customWidth="1"/>
-    <col min="7939" max="8192" width="9.140625" style="1"/>
-    <col min="8193" max="8193" width="11.5703125" style="1" customWidth="1"/>
-    <col min="8194" max="8194" width="36.5703125" style="1" customWidth="1"/>
-    <col min="8195" max="8448" width="9.140625" style="1"/>
-    <col min="8449" max="8449" width="11.5703125" style="1" customWidth="1"/>
-    <col min="8450" max="8450" width="36.5703125" style="1" customWidth="1"/>
-    <col min="8451" max="8704" width="9.140625" style="1"/>
-    <col min="8705" max="8705" width="11.5703125" style="1" customWidth="1"/>
-    <col min="8706" max="8706" width="36.5703125" style="1" customWidth="1"/>
-    <col min="8707" max="8960" width="9.140625" style="1"/>
-    <col min="8961" max="8961" width="11.5703125" style="1" customWidth="1"/>
-    <col min="8962" max="8962" width="36.5703125" style="1" customWidth="1"/>
-    <col min="8963" max="9216" width="9.140625" style="1"/>
-    <col min="9217" max="9217" width="11.5703125" style="1" customWidth="1"/>
-    <col min="9218" max="9218" width="36.5703125" style="1" customWidth="1"/>
-    <col min="9219" max="9472" width="9.140625" style="1"/>
-    <col min="9473" max="9473" width="11.5703125" style="1" customWidth="1"/>
-    <col min="9474" max="9474" width="36.5703125" style="1" customWidth="1"/>
-    <col min="9475" max="9728" width="9.140625" style="1"/>
-    <col min="9729" max="9729" width="11.5703125" style="1" customWidth="1"/>
-    <col min="9730" max="9730" width="36.5703125" style="1" customWidth="1"/>
-    <col min="9731" max="9984" width="9.140625" style="1"/>
-    <col min="9985" max="9985" width="11.5703125" style="1" customWidth="1"/>
-    <col min="9986" max="9986" width="36.5703125" style="1" customWidth="1"/>
-    <col min="9987" max="10240" width="9.140625" style="1"/>
-    <col min="10241" max="10241" width="11.5703125" style="1" customWidth="1"/>
-    <col min="10242" max="10242" width="36.5703125" style="1" customWidth="1"/>
-    <col min="10243" max="10496" width="9.140625" style="1"/>
-    <col min="10497" max="10497" width="11.5703125" style="1" customWidth="1"/>
-    <col min="10498" max="10498" width="36.5703125" style="1" customWidth="1"/>
-    <col min="10499" max="10752" width="9.140625" style="1"/>
-    <col min="10753" max="10753" width="11.5703125" style="1" customWidth="1"/>
-    <col min="10754" max="10754" width="36.5703125" style="1" customWidth="1"/>
-    <col min="10755" max="11008" width="9.140625" style="1"/>
-    <col min="11009" max="11009" width="11.5703125" style="1" customWidth="1"/>
-    <col min="11010" max="11010" width="36.5703125" style="1" customWidth="1"/>
-    <col min="11011" max="11264" width="9.140625" style="1"/>
-    <col min="11265" max="11265" width="11.5703125" style="1" customWidth="1"/>
-    <col min="11266" max="11266" width="36.5703125" style="1" customWidth="1"/>
-    <col min="11267" max="11520" width="9.140625" style="1"/>
-    <col min="11521" max="11521" width="11.5703125" style="1" customWidth="1"/>
-    <col min="11522" max="11522" width="36.5703125" style="1" customWidth="1"/>
-    <col min="11523" max="11776" width="9.140625" style="1"/>
-    <col min="11777" max="11777" width="11.5703125" style="1" customWidth="1"/>
-    <col min="11778" max="11778" width="36.5703125" style="1" customWidth="1"/>
-    <col min="11779" max="12032" width="9.140625" style="1"/>
-    <col min="12033" max="12033" width="11.5703125" style="1" customWidth="1"/>
-    <col min="12034" max="12034" width="36.5703125" style="1" customWidth="1"/>
-    <col min="12035" max="12288" width="9.140625" style="1"/>
-    <col min="12289" max="12289" width="11.5703125" style="1" customWidth="1"/>
-    <col min="12290" max="12290" width="36.5703125" style="1" customWidth="1"/>
-    <col min="12291" max="12544" width="9.140625" style="1"/>
-    <col min="12545" max="12545" width="11.5703125" style="1" customWidth="1"/>
-    <col min="12546" max="12546" width="36.5703125" style="1" customWidth="1"/>
-    <col min="12547" max="12800" width="9.140625" style="1"/>
-    <col min="12801" max="12801" width="11.5703125" style="1" customWidth="1"/>
-    <col min="12802" max="12802" width="36.5703125" style="1" customWidth="1"/>
-    <col min="12803" max="13056" width="9.140625" style="1"/>
-    <col min="13057" max="13057" width="11.5703125" style="1" customWidth="1"/>
-    <col min="13058" max="13058" width="36.5703125" style="1" customWidth="1"/>
-    <col min="13059" max="13312" width="9.140625" style="1"/>
-    <col min="13313" max="13313" width="11.5703125" style="1" customWidth="1"/>
-    <col min="13314" max="13314" width="36.5703125" style="1" customWidth="1"/>
-    <col min="13315" max="13568" width="9.140625" style="1"/>
-    <col min="13569" max="13569" width="11.5703125" style="1" customWidth="1"/>
-    <col min="13570" max="13570" width="36.5703125" style="1" customWidth="1"/>
-    <col min="13571" max="13824" width="9.140625" style="1"/>
-    <col min="13825" max="13825" width="11.5703125" style="1" customWidth="1"/>
-    <col min="13826" max="13826" width="36.5703125" style="1" customWidth="1"/>
-    <col min="13827" max="14080" width="9.140625" style="1"/>
-    <col min="14081" max="14081" width="11.5703125" style="1" customWidth="1"/>
-    <col min="14082" max="14082" width="36.5703125" style="1" customWidth="1"/>
-    <col min="14083" max="14336" width="9.140625" style="1"/>
-    <col min="14337" max="14337" width="11.5703125" style="1" customWidth="1"/>
-    <col min="14338" max="14338" width="36.5703125" style="1" customWidth="1"/>
-    <col min="14339" max="14592" width="9.140625" style="1"/>
-    <col min="14593" max="14593" width="11.5703125" style="1" customWidth="1"/>
-    <col min="14594" max="14594" width="36.5703125" style="1" customWidth="1"/>
-    <col min="14595" max="14848" width="9.140625" style="1"/>
-    <col min="14849" max="14849" width="11.5703125" style="1" customWidth="1"/>
-    <col min="14850" max="14850" width="36.5703125" style="1" customWidth="1"/>
-    <col min="14851" max="15104" width="9.140625" style="1"/>
-    <col min="15105" max="15105" width="11.5703125" style="1" customWidth="1"/>
-    <col min="15106" max="15106" width="36.5703125" style="1" customWidth="1"/>
-    <col min="15107" max="15360" width="9.140625" style="1"/>
-    <col min="15361" max="15361" width="11.5703125" style="1" customWidth="1"/>
-    <col min="15362" max="15362" width="36.5703125" style="1" customWidth="1"/>
-    <col min="15363" max="15616" width="9.140625" style="1"/>
-    <col min="15617" max="15617" width="11.5703125" style="1" customWidth="1"/>
-    <col min="15618" max="15618" width="36.5703125" style="1" customWidth="1"/>
-    <col min="15619" max="15872" width="9.140625" style="1"/>
-    <col min="15873" max="15873" width="11.5703125" style="1" customWidth="1"/>
-    <col min="15874" max="15874" width="36.5703125" style="1" customWidth="1"/>
-    <col min="15875" max="16128" width="9.140625" style="1"/>
-    <col min="16129" max="16129" width="11.5703125" style="1" customWidth="1"/>
-    <col min="16130" max="16130" width="36.5703125" style="1" customWidth="1"/>
-    <col min="16131" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.59765625" style="1" customWidth="1"/>
+    <col min="3" max="256" width="9.19921875" style="1"/>
+    <col min="257" max="257" width="11.59765625" style="1" customWidth="1"/>
+    <col min="258" max="258" width="36.59765625" style="1" customWidth="1"/>
+    <col min="259" max="512" width="9.19921875" style="1"/>
+    <col min="513" max="513" width="11.59765625" style="1" customWidth="1"/>
+    <col min="514" max="514" width="36.59765625" style="1" customWidth="1"/>
+    <col min="515" max="768" width="9.19921875" style="1"/>
+    <col min="769" max="769" width="11.59765625" style="1" customWidth="1"/>
+    <col min="770" max="770" width="36.59765625" style="1" customWidth="1"/>
+    <col min="771" max="1024" width="9.19921875" style="1"/>
+    <col min="1025" max="1025" width="11.59765625" style="1" customWidth="1"/>
+    <col min="1026" max="1026" width="36.59765625" style="1" customWidth="1"/>
+    <col min="1027" max="1280" width="9.19921875" style="1"/>
+    <col min="1281" max="1281" width="11.59765625" style="1" customWidth="1"/>
+    <col min="1282" max="1282" width="36.59765625" style="1" customWidth="1"/>
+    <col min="1283" max="1536" width="9.19921875" style="1"/>
+    <col min="1537" max="1537" width="11.59765625" style="1" customWidth="1"/>
+    <col min="1538" max="1538" width="36.59765625" style="1" customWidth="1"/>
+    <col min="1539" max="1792" width="9.19921875" style="1"/>
+    <col min="1793" max="1793" width="11.59765625" style="1" customWidth="1"/>
+    <col min="1794" max="1794" width="36.59765625" style="1" customWidth="1"/>
+    <col min="1795" max="2048" width="9.19921875" style="1"/>
+    <col min="2049" max="2049" width="11.59765625" style="1" customWidth="1"/>
+    <col min="2050" max="2050" width="36.59765625" style="1" customWidth="1"/>
+    <col min="2051" max="2304" width="9.19921875" style="1"/>
+    <col min="2305" max="2305" width="11.59765625" style="1" customWidth="1"/>
+    <col min="2306" max="2306" width="36.59765625" style="1" customWidth="1"/>
+    <col min="2307" max="2560" width="9.19921875" style="1"/>
+    <col min="2561" max="2561" width="11.59765625" style="1" customWidth="1"/>
+    <col min="2562" max="2562" width="36.59765625" style="1" customWidth="1"/>
+    <col min="2563" max="2816" width="9.19921875" style="1"/>
+    <col min="2817" max="2817" width="11.59765625" style="1" customWidth="1"/>
+    <col min="2818" max="2818" width="36.59765625" style="1" customWidth="1"/>
+    <col min="2819" max="3072" width="9.19921875" style="1"/>
+    <col min="3073" max="3073" width="11.59765625" style="1" customWidth="1"/>
+    <col min="3074" max="3074" width="36.59765625" style="1" customWidth="1"/>
+    <col min="3075" max="3328" width="9.19921875" style="1"/>
+    <col min="3329" max="3329" width="11.59765625" style="1" customWidth="1"/>
+    <col min="3330" max="3330" width="36.59765625" style="1" customWidth="1"/>
+    <col min="3331" max="3584" width="9.19921875" style="1"/>
+    <col min="3585" max="3585" width="11.59765625" style="1" customWidth="1"/>
+    <col min="3586" max="3586" width="36.59765625" style="1" customWidth="1"/>
+    <col min="3587" max="3840" width="9.19921875" style="1"/>
+    <col min="3841" max="3841" width="11.59765625" style="1" customWidth="1"/>
+    <col min="3842" max="3842" width="36.59765625" style="1" customWidth="1"/>
+    <col min="3843" max="4096" width="9.19921875" style="1"/>
+    <col min="4097" max="4097" width="11.59765625" style="1" customWidth="1"/>
+    <col min="4098" max="4098" width="36.59765625" style="1" customWidth="1"/>
+    <col min="4099" max="4352" width="9.19921875" style="1"/>
+    <col min="4353" max="4353" width="11.59765625" style="1" customWidth="1"/>
+    <col min="4354" max="4354" width="36.59765625" style="1" customWidth="1"/>
+    <col min="4355" max="4608" width="9.19921875" style="1"/>
+    <col min="4609" max="4609" width="11.59765625" style="1" customWidth="1"/>
+    <col min="4610" max="4610" width="36.59765625" style="1" customWidth="1"/>
+    <col min="4611" max="4864" width="9.19921875" style="1"/>
+    <col min="4865" max="4865" width="11.59765625" style="1" customWidth="1"/>
+    <col min="4866" max="4866" width="36.59765625" style="1" customWidth="1"/>
+    <col min="4867" max="5120" width="9.19921875" style="1"/>
+    <col min="5121" max="5121" width="11.59765625" style="1" customWidth="1"/>
+    <col min="5122" max="5122" width="36.59765625" style="1" customWidth="1"/>
+    <col min="5123" max="5376" width="9.19921875" style="1"/>
+    <col min="5377" max="5377" width="11.59765625" style="1" customWidth="1"/>
+    <col min="5378" max="5378" width="36.59765625" style="1" customWidth="1"/>
+    <col min="5379" max="5632" width="9.19921875" style="1"/>
+    <col min="5633" max="5633" width="11.59765625" style="1" customWidth="1"/>
+    <col min="5634" max="5634" width="36.59765625" style="1" customWidth="1"/>
+    <col min="5635" max="5888" width="9.19921875" style="1"/>
+    <col min="5889" max="5889" width="11.59765625" style="1" customWidth="1"/>
+    <col min="5890" max="5890" width="36.59765625" style="1" customWidth="1"/>
+    <col min="5891" max="6144" width="9.19921875" style="1"/>
+    <col min="6145" max="6145" width="11.59765625" style="1" customWidth="1"/>
+    <col min="6146" max="6146" width="36.59765625" style="1" customWidth="1"/>
+    <col min="6147" max="6400" width="9.19921875" style="1"/>
+    <col min="6401" max="6401" width="11.59765625" style="1" customWidth="1"/>
+    <col min="6402" max="6402" width="36.59765625" style="1" customWidth="1"/>
+    <col min="6403" max="6656" width="9.19921875" style="1"/>
+    <col min="6657" max="6657" width="11.59765625" style="1" customWidth="1"/>
+    <col min="6658" max="6658" width="36.59765625" style="1" customWidth="1"/>
+    <col min="6659" max="6912" width="9.19921875" style="1"/>
+    <col min="6913" max="6913" width="11.59765625" style="1" customWidth="1"/>
+    <col min="6914" max="6914" width="36.59765625" style="1" customWidth="1"/>
+    <col min="6915" max="7168" width="9.19921875" style="1"/>
+    <col min="7169" max="7169" width="11.59765625" style="1" customWidth="1"/>
+    <col min="7170" max="7170" width="36.59765625" style="1" customWidth="1"/>
+    <col min="7171" max="7424" width="9.19921875" style="1"/>
+    <col min="7425" max="7425" width="11.59765625" style="1" customWidth="1"/>
+    <col min="7426" max="7426" width="36.59765625" style="1" customWidth="1"/>
+    <col min="7427" max="7680" width="9.19921875" style="1"/>
+    <col min="7681" max="7681" width="11.59765625" style="1" customWidth="1"/>
+    <col min="7682" max="7682" width="36.59765625" style="1" customWidth="1"/>
+    <col min="7683" max="7936" width="9.19921875" style="1"/>
+    <col min="7937" max="7937" width="11.59765625" style="1" customWidth="1"/>
+    <col min="7938" max="7938" width="36.59765625" style="1" customWidth="1"/>
+    <col min="7939" max="8192" width="9.19921875" style="1"/>
+    <col min="8193" max="8193" width="11.59765625" style="1" customWidth="1"/>
+    <col min="8194" max="8194" width="36.59765625" style="1" customWidth="1"/>
+    <col min="8195" max="8448" width="9.19921875" style="1"/>
+    <col min="8449" max="8449" width="11.59765625" style="1" customWidth="1"/>
+    <col min="8450" max="8450" width="36.59765625" style="1" customWidth="1"/>
+    <col min="8451" max="8704" width="9.19921875" style="1"/>
+    <col min="8705" max="8705" width="11.59765625" style="1" customWidth="1"/>
+    <col min="8706" max="8706" width="36.59765625" style="1" customWidth="1"/>
+    <col min="8707" max="8960" width="9.19921875" style="1"/>
+    <col min="8961" max="8961" width="11.59765625" style="1" customWidth="1"/>
+    <col min="8962" max="8962" width="36.59765625" style="1" customWidth="1"/>
+    <col min="8963" max="9216" width="9.19921875" style="1"/>
+    <col min="9217" max="9217" width="11.59765625" style="1" customWidth="1"/>
+    <col min="9218" max="9218" width="36.59765625" style="1" customWidth="1"/>
+    <col min="9219" max="9472" width="9.19921875" style="1"/>
+    <col min="9473" max="9473" width="11.59765625" style="1" customWidth="1"/>
+    <col min="9474" max="9474" width="36.59765625" style="1" customWidth="1"/>
+    <col min="9475" max="9728" width="9.19921875" style="1"/>
+    <col min="9729" max="9729" width="11.59765625" style="1" customWidth="1"/>
+    <col min="9730" max="9730" width="36.59765625" style="1" customWidth="1"/>
+    <col min="9731" max="9984" width="9.19921875" style="1"/>
+    <col min="9985" max="9985" width="11.59765625" style="1" customWidth="1"/>
+    <col min="9986" max="9986" width="36.59765625" style="1" customWidth="1"/>
+    <col min="9987" max="10240" width="9.19921875" style="1"/>
+    <col min="10241" max="10241" width="11.59765625" style="1" customWidth="1"/>
+    <col min="10242" max="10242" width="36.59765625" style="1" customWidth="1"/>
+    <col min="10243" max="10496" width="9.19921875" style="1"/>
+    <col min="10497" max="10497" width="11.59765625" style="1" customWidth="1"/>
+    <col min="10498" max="10498" width="36.59765625" style="1" customWidth="1"/>
+    <col min="10499" max="10752" width="9.19921875" style="1"/>
+    <col min="10753" max="10753" width="11.59765625" style="1" customWidth="1"/>
+    <col min="10754" max="10754" width="36.59765625" style="1" customWidth="1"/>
+    <col min="10755" max="11008" width="9.19921875" style="1"/>
+    <col min="11009" max="11009" width="11.59765625" style="1" customWidth="1"/>
+    <col min="11010" max="11010" width="36.59765625" style="1" customWidth="1"/>
+    <col min="11011" max="11264" width="9.19921875" style="1"/>
+    <col min="11265" max="11265" width="11.59765625" style="1" customWidth="1"/>
+    <col min="11266" max="11266" width="36.59765625" style="1" customWidth="1"/>
+    <col min="11267" max="11520" width="9.19921875" style="1"/>
+    <col min="11521" max="11521" width="11.59765625" style="1" customWidth="1"/>
+    <col min="11522" max="11522" width="36.59765625" style="1" customWidth="1"/>
+    <col min="11523" max="11776" width="9.19921875" style="1"/>
+    <col min="11777" max="11777" width="11.59765625" style="1" customWidth="1"/>
+    <col min="11778" max="11778" width="36.59765625" style="1" customWidth="1"/>
+    <col min="11779" max="12032" width="9.19921875" style="1"/>
+    <col min="12033" max="12033" width="11.59765625" style="1" customWidth="1"/>
+    <col min="12034" max="12034" width="36.59765625" style="1" customWidth="1"/>
+    <col min="12035" max="12288" width="9.19921875" style="1"/>
+    <col min="12289" max="12289" width="11.59765625" style="1" customWidth="1"/>
+    <col min="12290" max="12290" width="36.59765625" style="1" customWidth="1"/>
+    <col min="12291" max="12544" width="9.19921875" style="1"/>
+    <col min="12545" max="12545" width="11.59765625" style="1" customWidth="1"/>
+    <col min="12546" max="12546" width="36.59765625" style="1" customWidth="1"/>
+    <col min="12547" max="12800" width="9.19921875" style="1"/>
+    <col min="12801" max="12801" width="11.59765625" style="1" customWidth="1"/>
+    <col min="12802" max="12802" width="36.59765625" style="1" customWidth="1"/>
+    <col min="12803" max="13056" width="9.19921875" style="1"/>
+    <col min="13057" max="13057" width="11.59765625" style="1" customWidth="1"/>
+    <col min="13058" max="13058" width="36.59765625" style="1" customWidth="1"/>
+    <col min="13059" max="13312" width="9.19921875" style="1"/>
+    <col min="13313" max="13313" width="11.59765625" style="1" customWidth="1"/>
+    <col min="13314" max="13314" width="36.59765625" style="1" customWidth="1"/>
+    <col min="13315" max="13568" width="9.19921875" style="1"/>
+    <col min="13569" max="13569" width="11.59765625" style="1" customWidth="1"/>
+    <col min="13570" max="13570" width="36.59765625" style="1" customWidth="1"/>
+    <col min="13571" max="13824" width="9.19921875" style="1"/>
+    <col min="13825" max="13825" width="11.59765625" style="1" customWidth="1"/>
+    <col min="13826" max="13826" width="36.59765625" style="1" customWidth="1"/>
+    <col min="13827" max="14080" width="9.19921875" style="1"/>
+    <col min="14081" max="14081" width="11.59765625" style="1" customWidth="1"/>
+    <col min="14082" max="14082" width="36.59765625" style="1" customWidth="1"/>
+    <col min="14083" max="14336" width="9.19921875" style="1"/>
+    <col min="14337" max="14337" width="11.59765625" style="1" customWidth="1"/>
+    <col min="14338" max="14338" width="36.59765625" style="1" customWidth="1"/>
+    <col min="14339" max="14592" width="9.19921875" style="1"/>
+    <col min="14593" max="14593" width="11.59765625" style="1" customWidth="1"/>
+    <col min="14594" max="14594" width="36.59765625" style="1" customWidth="1"/>
+    <col min="14595" max="14848" width="9.19921875" style="1"/>
+    <col min="14849" max="14849" width="11.59765625" style="1" customWidth="1"/>
+    <col min="14850" max="14850" width="36.59765625" style="1" customWidth="1"/>
+    <col min="14851" max="15104" width="9.19921875" style="1"/>
+    <col min="15105" max="15105" width="11.59765625" style="1" customWidth="1"/>
+    <col min="15106" max="15106" width="36.59765625" style="1" customWidth="1"/>
+    <col min="15107" max="15360" width="9.19921875" style="1"/>
+    <col min="15361" max="15361" width="11.59765625" style="1" customWidth="1"/>
+    <col min="15362" max="15362" width="36.59765625" style="1" customWidth="1"/>
+    <col min="15363" max="15616" width="9.19921875" style="1"/>
+    <col min="15617" max="15617" width="11.59765625" style="1" customWidth="1"/>
+    <col min="15618" max="15618" width="36.59765625" style="1" customWidth="1"/>
+    <col min="15619" max="15872" width="9.19921875" style="1"/>
+    <col min="15873" max="15873" width="11.59765625" style="1" customWidth="1"/>
+    <col min="15874" max="15874" width="36.59765625" style="1" customWidth="1"/>
+    <col min="15875" max="16128" width="9.19921875" style="1"/>
+    <col min="16129" max="16129" width="11.59765625" style="1" customWidth="1"/>
+    <col min="16130" max="16130" width="36.59765625" style="1" customWidth="1"/>
+    <col min="16131" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>120</v>
       </c>
@@ -5007,7 +4648,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
@@ -5015,7 +4656,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>124</v>
       </c>
@@ -5023,7 +4664,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>126</v>
       </c>
@@ -5031,7 +4672,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>128</v>
       </c>
@@ -5039,7 +4680,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>130</v>
       </c>
@@ -5047,7 +4688,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>132</v>
       </c>
@@ -5055,7 +4696,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>134</v>
       </c>
@@ -5063,7 +4704,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>136</v>
       </c>
@@ -5071,7 +4712,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>138</v>
       </c>
@@ -5079,7 +4720,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -5087,7 +4728,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>141</v>
       </c>
@@ -5095,7 +4736,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>143</v>
       </c>
@@ -5103,7 +4744,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>145</v>
       </c>

</xml_diff>